<commit_message>
update In Class Demonstration
</commit_message>
<xml_diff>
--- a/Projects/Federal Reserve Data/Aggregated C&A  Diff-in-DiffDAGOLS 2005-12-31 to 2008-09-30.xlsx
+++ b/Projects/Federal Reserve Data/Aggregated C&A  Diff-in-DiffDAGOLS 2005-12-31 to 2008-09-30.xlsx
@@ -16,16 +16,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
-    <t>C Diff-in-Diff</t>
-  </si>
-  <si>
-    <t>LF Diff-in-Diff</t>
-  </si>
-  <si>
-    <t>FFR Diff-in-Diff</t>
-  </si>
-  <si>
-    <t>A Diff-in-Diff</t>
+    <t>C</t>
+  </si>
+  <si>
+    <t>LF</t>
+  </si>
+  <si>
+    <t>FFR</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
   <si>
     <t>Constant</t>
@@ -34,52 +34,52 @@
     <t>r2_adj</t>
   </si>
   <si>
-    <t>-0.165</t>
-  </si>
-  <si>
-    <t>-1.594***</t>
-  </si>
-  <si>
-    <t>12.885</t>
-  </si>
-  <si>
-    <t>-4.285***</t>
-  </si>
-  <si>
-    <t>-0.036</t>
-  </si>
-  <si>
-    <t>0.505*</t>
-  </si>
-  <si>
-    <t>-18.697**</t>
-  </si>
-  <si>
-    <t>-0.113</t>
-  </si>
-  <si>
-    <t>-0.289***</t>
-  </si>
-  <si>
-    <t>0.421*</t>
-  </si>
-  <si>
-    <t>12.716*</t>
-  </si>
-  <si>
-    <t>-1.872***</t>
-  </si>
-  <si>
-    <t>0.003</t>
-  </si>
-  <si>
-    <t>-0.022**</t>
-  </si>
-  <si>
-    <t>0.018*</t>
-  </si>
-  <si>
-    <t>0.021</t>
+    <t>-0.368</t>
+  </si>
+  <si>
+    <t>-0.158</t>
+  </si>
+  <si>
+    <t>-3.273</t>
+  </si>
+  <si>
+    <t>-0.685</t>
+  </si>
+  <si>
+    <t>-0.042</t>
+  </si>
+  <si>
+    <t>0.408***</t>
+  </si>
+  <si>
+    <t>-9.409*</t>
+  </si>
+  <si>
+    <t>-0.431*</t>
+  </si>
+  <si>
+    <t>-0.044</t>
+  </si>
+  <si>
+    <t>0.998***</t>
+  </si>
+  <si>
+    <t>-5.344</t>
+  </si>
+  <si>
+    <t>-0.429</t>
+  </si>
+  <si>
+    <t>-0.001</t>
+  </si>
+  <si>
+    <t>-0.016*</t>
+  </si>
+  <si>
+    <t>-0.004</t>
+  </si>
+  <si>
+    <t>-0.021**</t>
   </si>
 </sst>
 </file>
@@ -535,16 +535,16 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.61</v>
+        <v>-0.01</v>
       </c>
       <c r="C7">
-        <v>0.59</v>
+        <v>0.63</v>
       </c>
       <c r="D7">
-        <v>0.68</v>
+        <v>0.57</v>
       </c>
       <c r="E7">
-        <v>0.39</v>
+        <v>0.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>